<commit_message>
wording for full/complete fixed in CLAN
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Documents/GitHub/CLAN_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E4B80F-2CA1-9D44-B9DA-07034734FEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8008085C-1B32-064B-AEA2-0070252413CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="1240" windowWidth="26840" windowHeight="15940" xr2:uid="{FB669BDA-7798-9640-B2B9-EABE7DDFC01C}"/>
+    <workbookView xWindow="3400" yWindow="1220" windowWidth="26840" windowHeight="15940" xr2:uid="{FB669BDA-7798-9640-B2B9-EABE7DDFC01C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,9 +284,6 @@
     <t>Outcome</t>
   </si>
   <si>
-    <t>Full</t>
-  </si>
-  <si>
     <t>Cons/AE</t>
   </si>
   <si>
@@ -299,10 +296,13 @@
     <t>HH Rev</t>
   </si>
   <si>
-    <t>Pool (Cap &amp; Full)</t>
+    <t>Label</t>
   </si>
   <si>
-    <t>Label</t>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Pool (Cap &amp; Complete)</t>
   </si>
 </sst>
 </file>
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648B546F-8C97-294C-8991-7BD4B2B32DAC}">
   <dimension ref="A1:Y211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="J122" sqref="J122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>80</v>
@@ -792,10 +792,10 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
         <v>82</v>
-      </c>
-      <c r="D2" t="s">
-        <v>83</v>
       </c>
       <c r="E2" s="3">
         <v>3.9568345323740997E-2</v>
@@ -869,10 +869,10 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
         <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>83</v>
       </c>
       <c r="E3" s="3">
         <v>0.21742428634851699</v>
@@ -946,10 +946,10 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
       </c>
       <c r="E4" s="3">
         <v>17.438486976774598</v>
@@ -1023,10 +1023,10 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
         <v>82</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
       </c>
       <c r="E5" s="3">
         <v>0.383693045563549</v>
@@ -1100,10 +1100,10 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
         <v>82</v>
-      </c>
-      <c r="D6" t="s">
-        <v>83</v>
       </c>
       <c r="E6" s="3">
         <v>8.1175059952038406</v>
@@ -1177,10 +1177,10 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
         <v>82</v>
-      </c>
-      <c r="D7" t="s">
-        <v>83</v>
       </c>
       <c r="E7" s="3">
         <v>36.405275779376502</v>
@@ -1254,10 +1254,10 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
         <v>82</v>
-      </c>
-      <c r="D8" t="s">
-        <v>83</v>
       </c>
       <c r="E8" s="3">
         <v>0.694244604316547</v>
@@ -1331,10 +1331,10 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
         <v>82</v>
-      </c>
-      <c r="D9" t="s">
-        <v>83</v>
       </c>
       <c r="E9" s="3">
         <v>0.86690647482014405</v>
@@ -1408,10 +1408,10 @@
         <v>39</v>
       </c>
       <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
         <v>82</v>
-      </c>
-      <c r="D10" t="s">
-        <v>83</v>
       </c>
       <c r="E10" s="3">
         <v>1.3189448441247E-2</v>
@@ -1485,10 +1485,10 @@
         <v>41</v>
       </c>
       <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
         <v>82</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
       </c>
       <c r="E11" s="3">
         <v>0.10431654676259</v>
@@ -1562,10 +1562,10 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" t="s">
         <v>82</v>
-      </c>
-      <c r="D12" t="s">
-        <v>83</v>
       </c>
       <c r="E12" s="3">
         <v>5.7105148978412297E-2</v>
@@ -1639,10 +1639,10 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
         <v>82</v>
-      </c>
-      <c r="D13" t="s">
-        <v>83</v>
       </c>
       <c r="E13" s="3">
         <v>2.0383693045563499E-2</v>
@@ -1716,10 +1716,10 @@
         <v>47</v>
       </c>
       <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" t="s">
         <v>82</v>
-      </c>
-      <c r="D14" t="s">
-        <v>83</v>
       </c>
       <c r="E14" s="3">
         <v>15.100007457408999</v>
@@ -1793,10 +1793,10 @@
         <v>49</v>
       </c>
       <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
         <v>82</v>
-      </c>
-      <c r="D15" t="s">
-        <v>83</v>
       </c>
       <c r="E15" s="3">
         <v>57.429256594724201</v>
@@ -1870,10 +1870,10 @@
         <v>51</v>
       </c>
       <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
         <v>82</v>
-      </c>
-      <c r="D16" t="s">
-        <v>83</v>
       </c>
       <c r="E16" s="3">
         <v>6.4693825373010702E-2</v>
@@ -1947,10 +1947,10 @@
         <v>53</v>
       </c>
       <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" t="s">
         <v>82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>83</v>
       </c>
       <c r="E17" s="3">
         <v>6.4967557318604693E-2</v>
@@ -2024,10 +2024,10 @@
         <v>55</v>
       </c>
       <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
         <v>82</v>
-      </c>
-      <c r="D18" t="s">
-        <v>83</v>
       </c>
       <c r="E18" s="3">
         <v>398.773079058669</v>
@@ -2101,10 +2101,10 @@
         <v>57</v>
       </c>
       <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
         <v>82</v>
-      </c>
-      <c r="D19" t="s">
-        <v>83</v>
       </c>
       <c r="E19" s="3">
         <v>0.79736211031175097</v>
@@ -2178,10 +2178,10 @@
         <v>59</v>
       </c>
       <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" t="s">
         <v>82</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
       </c>
       <c r="E20" s="3">
         <v>0.37290167865707402</v>
@@ -2255,10 +2255,10 @@
         <v>61</v>
       </c>
       <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
       </c>
       <c r="E21" s="3">
         <v>4.4364508393285401E-2</v>
@@ -2332,10 +2332,10 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
         <v>82</v>
-      </c>
-      <c r="D22" t="s">
-        <v>83</v>
       </c>
       <c r="E22" s="3">
         <v>17.2904117202444</v>
@@ -2409,10 +2409,10 @@
         <v>65</v>
       </c>
       <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" t="s">
         <v>82</v>
-      </c>
-      <c r="D23" t="s">
-        <v>83</v>
       </c>
       <c r="E23" s="3">
         <v>0.21942446043165501</v>
@@ -2486,10 +2486,10 @@
         <v>67</v>
       </c>
       <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" t="s">
         <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
       </c>
       <c r="E24" s="3">
         <v>0.99931942233570104</v>
@@ -2563,10 +2563,10 @@
         <v>69</v>
       </c>
       <c r="C25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" t="s">
         <v>82</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
       </c>
       <c r="E25" s="3">
         <v>0.811148985744927</v>
@@ -2640,10 +2640,10 @@
         <v>71</v>
       </c>
       <c r="C26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
         <v>82</v>
-      </c>
-      <c r="D26" t="s">
-        <v>83</v>
       </c>
       <c r="E26" s="3">
         <v>-0.38890047118568</v>
@@ -2717,10 +2717,10 @@
         <v>72</v>
       </c>
       <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
         <v>82</v>
-      </c>
-      <c r="D27" t="s">
-        <v>83</v>
       </c>
       <c r="E27" s="3">
         <v>0.22661870503597101</v>
@@ -2794,10 +2794,10 @@
         <v>73</v>
       </c>
       <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" t="s">
-        <v>83</v>
       </c>
       <c r="E28" s="3">
         <v>0.27458033573141499</v>
@@ -2871,10 +2871,10 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
         <v>82</v>
-      </c>
-      <c r="D29" t="s">
-        <v>83</v>
       </c>
       <c r="E29" s="3">
         <v>0.25779376498800999</v>
@@ -2948,10 +2948,10 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" t="s">
         <v>82</v>
-      </c>
-      <c r="D30" t="s">
-        <v>83</v>
       </c>
       <c r="E30" s="3">
         <v>0.38489208633093502</v>
@@ -3025,10 +3025,10 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" t="s">
         <v>82</v>
-      </c>
-      <c r="D31" t="s">
-        <v>83</v>
       </c>
       <c r="E31" s="3">
         <v>0.35131894484412501</v>
@@ -3102,10 +3102,10 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="3">
         <v>1.3189448441247E-2</v>
@@ -3179,10 +3179,10 @@
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="3">
         <v>-1.73785793518243E-3</v>
@@ -3256,10 +3256,10 @@
         <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" s="3">
         <v>12.2996108413314</v>
@@ -3333,10 +3333,10 @@
         <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="3">
         <v>0.13549160671462801</v>
@@ -3410,10 +3410,10 @@
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="3">
         <v>8.8141486810551495</v>
@@ -3487,10 +3487,10 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E37" s="3">
         <v>35.272182254196601</v>
@@ -3564,10 +3564,10 @@
         <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" s="3">
         <v>0.12350119904076701</v>
@@ -3641,10 +3641,10 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E39" s="3">
         <v>0.94124700239808201</v>
@@ -3718,10 +3718,10 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
@@ -3795,10 +3795,10 @@
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41" s="3">
         <v>5.63549160671463E-2</v>
@@ -3872,10 +3872,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E42" s="3">
         <v>2.1570012509393999E-2</v>
@@ -3949,10 +3949,10 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" s="3">
         <v>1.55875299760192E-2</v>
@@ -4026,10 +4026,10 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E44" s="3">
         <v>14.0370250341737</v>
@@ -4103,10 +4103,10 @@
         <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E45" s="3">
         <v>54.070743405275799</v>
@@ -4180,10 +4180,10 @@
         <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E46" s="3">
         <v>4.3230917221002203E-2</v>
@@ -4257,10 +4257,10 @@
         <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E47" s="3">
         <v>0.11916598525374</v>
@@ -4334,10 +4334,10 @@
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E48" s="3">
         <v>205.77510939451801</v>
@@ -4411,10 +4411,10 @@
         <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E49" s="3">
         <v>0.92206235011990401</v>
@@ -4488,10 +4488,10 @@
         <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E50" s="3">
         <v>0.37769784172661902</v>
@@ -4565,10 +4565,10 @@
         <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E51" s="3">
         <v>1.07913669064748E-2</v>
@@ -4642,10 +4642,10 @@
         <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E52" s="3">
         <v>10.2661437150672</v>
@@ -4719,10 +4719,10 @@
         <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E53" s="3">
         <v>0.207434052757794</v>
@@ -4796,10 +4796,10 @@
         <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E54" s="3">
         <v>0.87373747166281901</v>
@@ -4873,10 +4873,10 @@
         <v>69</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E55" s="3">
         <v>0.71393699334360405</v>
@@ -4950,10 +4950,10 @@
         <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E56" s="3">
         <v>-0.52048391479176903</v>
@@ -5027,10 +5027,10 @@
         <v>72</v>
       </c>
       <c r="C57" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E57" s="3">
         <v>0.18105515587529999</v>
@@ -5104,10 +5104,10 @@
         <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E58" s="3">
         <v>0.17146282973621099</v>
@@ -5181,10 +5181,10 @@
         <v>75</v>
       </c>
       <c r="C59" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E59" s="3">
         <v>0.31294964028777</v>
@@ -5258,10 +5258,10 @@
         <v>77</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E60" s="3">
         <v>0.50719424460431695</v>
@@ -5335,10 +5335,10 @@
         <v>79</v>
       </c>
       <c r="C61" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E61" s="3">
         <v>0.17625899280575499</v>
@@ -5412,10 +5412,10 @@
         <v>23</v>
       </c>
       <c r="C62" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E62" s="3">
         <v>5.89622641509434E-3</v>
@@ -5489,10 +5489,10 @@
         <v>25</v>
       </c>
       <c r="C63" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E63" s="3">
         <v>4.3345027731362E-2</v>
@@ -5566,10 +5566,10 @@
         <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E64" s="3">
         <v>8.2430191090152594</v>
@@ -5643,10 +5643,10 @@
         <v>29</v>
       </c>
       <c r="C65" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E65" s="3">
         <v>7.19339622641509E-2</v>
@@ -5720,10 +5720,10 @@
         <v>31</v>
       </c>
       <c r="C66" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E66" s="3">
         <v>8.8856132075471699</v>
@@ -5797,10 +5797,10 @@
         <v>33</v>
       </c>
       <c r="C67" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E67" s="3">
         <v>34.728773584905703</v>
@@ -5874,10 +5874,10 @@
         <v>35</v>
       </c>
       <c r="C68" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E68" s="3">
         <v>5.0707547169811303E-2</v>
@@ -5951,10 +5951,10 @@
         <v>37</v>
       </c>
       <c r="C69" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E69" s="3">
         <v>0.93278301886792403</v>
@@ -6028,10 +6028,10 @@
         <v>39</v>
       </c>
       <c r="C70" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E70" s="3">
         <v>0</v>
@@ -6105,10 +6105,10 @@
         <v>41</v>
       </c>
       <c r="C71" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E71" s="3">
         <v>6.4858490566037694E-2</v>
@@ -6182,10 +6182,10 @@
         <v>43</v>
       </c>
       <c r="C72" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E72" s="3">
         <v>0.12673723473617801</v>
@@ -6259,10 +6259,10 @@
         <v>45</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E73" s="3">
         <v>3.5377358490566E-3</v>
@@ -6336,10 +6336,10 @@
         <v>47</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E74" s="3">
         <v>13.1354355410423</v>
@@ -6413,10 +6413,10 @@
         <v>49</v>
       </c>
       <c r="C75" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E75" s="3">
         <v>46.3867924528302</v>
@@ -6490,10 +6490,10 @@
         <v>51</v>
       </c>
       <c r="C76" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E76" s="3">
         <v>4.1735293784064598E-2</v>
@@ -6567,10 +6567,10 @@
         <v>53</v>
       </c>
       <c r="C77" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E77" s="3">
         <v>0.12894841599858001</v>
@@ -6644,10 +6644,10 @@
         <v>55</v>
       </c>
       <c r="C78" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E78" s="3">
         <v>182.47648462529099</v>
@@ -6721,10 +6721,10 @@
         <v>57</v>
       </c>
       <c r="C79" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E79" s="3">
         <v>0.95872641509433998</v>
@@ -6798,10 +6798,10 @@
         <v>59</v>
       </c>
       <c r="C80" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E80" s="3">
         <v>0.35259433962264197</v>
@@ -6875,10 +6875,10 @@
         <v>61</v>
       </c>
       <c r="C81" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E81" s="3">
         <v>3.5377358490566E-3</v>
@@ -6952,10 +6952,10 @@
         <v>63</v>
       </c>
       <c r="C82" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E82" s="3">
         <v>10.610788178331401</v>
@@ -7029,10 +7029,10 @@
         <v>65</v>
       </c>
       <c r="C83" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E83" s="3">
         <v>0.160377358490566</v>
@@ -7106,10 +7106,10 @@
         <v>67</v>
       </c>
       <c r="C84" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E84" s="3">
         <v>0.86935425244869202</v>
@@ -7183,10 +7183,10 @@
         <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E85" s="3">
         <v>0.61074655324183302</v>
@@ -7260,10 +7260,10 @@
         <v>71</v>
       </c>
       <c r="C86" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E86" s="3">
         <v>-0.52067419972472795</v>
@@ -7337,10 +7337,10 @@
         <v>72</v>
       </c>
       <c r="C87" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E87" s="3">
         <v>9.3160377358490601E-2</v>
@@ -7414,10 +7414,10 @@
         <v>73</v>
       </c>
       <c r="C88" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E88" s="3">
         <v>0.107311320754717</v>
@@ -7491,10 +7491,10 @@
         <v>75</v>
       </c>
       <c r="C89" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E89" s="3">
         <v>0.258254716981132</v>
@@ -7568,10 +7568,10 @@
         <v>77</v>
       </c>
       <c r="C90" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E90" s="3">
         <v>0.61438679245283001</v>
@@ -7645,10 +7645,10 @@
         <v>79</v>
       </c>
       <c r="C91" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E91" s="3">
         <v>0.12382075471698099</v>
@@ -7722,10 +7722,10 @@
         <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E92" s="3">
         <v>1.06132075471698E-2</v>
@@ -7799,10 +7799,10 @@
         <v>25</v>
       </c>
       <c r="C93" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E93" s="3">
         <v>6.7503922695803598E-3</v>
@@ -7876,10 +7876,10 @@
         <v>27</v>
       </c>
       <c r="C94" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E94" s="3">
         <v>11.1653581680862</v>
@@ -7953,10 +7953,10 @@
         <v>29</v>
       </c>
       <c r="C95" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E95" s="3">
         <v>0.102594339622642</v>
@@ -8030,10 +8030,10 @@
         <v>31</v>
       </c>
       <c r="C96" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E96" s="3">
         <v>8.8832547169811296</v>
@@ -8107,10 +8107,10 @@
         <v>33</v>
       </c>
       <c r="C97" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E97" s="3">
         <v>35.227594339622598</v>
@@ -8184,10 +8184,10 @@
         <v>35</v>
       </c>
       <c r="C98" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E98" s="3">
         <v>0.112028301886792</v>
@@ -8261,10 +8261,10 @@
         <v>37</v>
       </c>
       <c r="C99" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E99" s="3">
         <v>0.93042452830188704</v>
@@ -8338,10 +8338,10 @@
         <v>39</v>
       </c>
       <c r="C100" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E100" s="3">
         <v>0</v>
@@ -8415,10 +8415,10 @@
         <v>41</v>
       </c>
       <c r="C101" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E101" s="3">
         <v>6.7216981132075498E-2</v>
@@ -8492,10 +8492,10 @@
         <v>43</v>
       </c>
       <c r="C102" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E102" s="3">
         <v>0.102587189736231</v>
@@ -8569,10 +8569,10 @@
         <v>45</v>
       </c>
       <c r="C103" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E103" s="3">
         <v>8.2547169811320806E-3</v>
@@ -8646,10 +8646,10 @@
         <v>47</v>
       </c>
       <c r="C104" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E104" s="3">
         <v>13.4068636473735</v>
@@ -8723,10 +8723,10 @@
         <v>49</v>
       </c>
       <c r="C105" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E105" s="3">
         <v>49.071933962264197</v>
@@ -8800,10 +8800,10 @@
         <v>51</v>
       </c>
       <c r="C106" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E106" s="3">
         <v>4.4246120529934603E-2</v>
@@ -8877,10 +8877,10 @@
         <v>53</v>
       </c>
       <c r="C107" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E107" s="3">
         <v>0.11729874169917399</v>
@@ -8954,10 +8954,10 @@
         <v>55</v>
       </c>
       <c r="C108" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E108" s="3">
         <v>189.63563452348799</v>
@@ -9031,10 +9031,10 @@
         <v>57</v>
       </c>
       <c r="C109" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E109" s="3">
         <v>0.94221698113207597</v>
@@ -9108,10 +9108,10 @@
         <v>59</v>
       </c>
       <c r="C110" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E110" s="3">
         <v>0.35495283018867901</v>
@@ -9185,10 +9185,10 @@
         <v>61</v>
       </c>
       <c r="C111" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E111" s="3">
         <v>1.06132075471698E-2</v>
@@ -9262,10 +9262,10 @@
         <v>63</v>
       </c>
       <c r="C112" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E112" s="3">
         <v>9.9152792385726602</v>
@@ -9339,10 +9339,10 @@
         <v>65</v>
       </c>
       <c r="C113" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E113" s="3">
         <v>0.18985849056603801</v>
@@ -9416,10 +9416,10 @@
         <v>67</v>
       </c>
       <c r="C114" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E114" s="3">
         <v>0.83741318474892701</v>
@@ -9493,10 +9493,10 @@
         <v>69</v>
       </c>
       <c r="C115" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E115" s="3">
         <v>0.62825974443200405</v>
@@ -9570,10 +9570,10 @@
         <v>71</v>
       </c>
       <c r="C116" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E116" s="3">
         <v>-0.58836795528911301</v>
@@ -9647,10 +9647,10 @@
         <v>72</v>
       </c>
       <c r="C117" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E117" s="3">
         <v>0.13089622641509399</v>
@@ -9724,10 +9724,10 @@
         <v>73</v>
       </c>
       <c r="C118" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E118" s="3">
         <v>0.14033018867924499</v>
@@ -9801,10 +9801,10 @@
         <v>75</v>
       </c>
       <c r="C119" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E119" s="3">
         <v>0.27830188679245299</v>
@@ -9878,10 +9878,10 @@
         <v>77</v>
       </c>
       <c r="C120" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E120" s="3">
         <v>0.60731132075471705</v>
@@ -9955,10 +9955,10 @@
         <v>79</v>
       </c>
       <c r="C121" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E121" s="3">
         <v>0.112028301886792</v>
@@ -10032,10 +10032,10 @@
         <v>23</v>
       </c>
       <c r="C122" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E122" s="3">
         <v>8.8852988691437793E-3</v>
@@ -10109,10 +10109,10 @@
         <v>25</v>
       </c>
       <c r="C123" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E123" s="3">
         <v>2.6227295905513801E-2</v>
@@ -10186,10 +10186,10 @@
         <v>27</v>
       </c>
       <c r="C124" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E124" s="3">
         <v>12.6983609898181</v>
@@ -10263,10 +10263,10 @@
         <v>29</v>
       </c>
       <c r="C125" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E125" s="3">
         <v>0.123586429725363</v>
@@ -10340,10 +10340,10 @@
         <v>31</v>
       </c>
       <c r="C126" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E126" s="3">
         <v>8.5096930533117892</v>
@@ -10417,10 +10417,10 @@
         <v>33</v>
       </c>
       <c r="C127" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E127" s="3">
         <v>35.735864297253599</v>
@@ -10494,10 +10494,10 @@
         <v>35</v>
       </c>
       <c r="C128" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E128" s="3">
         <v>8.6429725363489501E-2</v>
@@ -10571,10 +10571,10 @@
         <v>37</v>
       </c>
       <c r="C129" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E129" s="3">
         <v>0.95234248788368303</v>
@@ -10648,10 +10648,10 @@
         <v>39</v>
       </c>
       <c r="C130" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E130" s="3">
         <v>0</v>
@@ -10725,10 +10725,10 @@
         <v>41</v>
       </c>
       <c r="C131" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E131" s="3">
         <v>4.60420032310178E-2</v>
@@ -10802,10 +10802,10 @@
         <v>43</v>
       </c>
       <c r="C132" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E132" s="3">
         <v>-4.00549178621062E-3</v>
@@ -10879,10 +10879,10 @@
         <v>45</v>
       </c>
       <c r="C133" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E133" s="3">
         <v>8.8852988691437793E-3</v>
@@ -10956,10 +10956,10 @@
         <v>47</v>
       </c>
       <c r="C134" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E134" s="3">
         <v>14.3696423466338</v>
@@ -11033,10 +11033,10 @@
         <v>49</v>
       </c>
       <c r="C135" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E135" s="3">
         <v>52.5444264943457</v>
@@ -11110,10 +11110,10 @@
         <v>51</v>
       </c>
       <c r="C136" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E136" s="3">
         <v>3.9280076180201101E-2</v>
@@ -11187,10 +11187,10 @@
         <v>53</v>
       </c>
       <c r="C137" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E137" s="3">
         <v>0.10700162516862501</v>
@@ -11264,10 +11264,10 @@
         <v>55</v>
       </c>
       <c r="C138" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E138" s="3">
         <v>211.78333485075601</v>
@@ -11341,10 +11341,10 @@
         <v>57</v>
       </c>
       <c r="C139" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E139" s="3">
         <v>0.93457189014539599</v>
@@ -11418,10 +11418,10 @@
         <v>59</v>
       </c>
       <c r="C140" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E140" s="3">
         <v>0.40468497576736701</v>
@@ -11495,10 +11495,10 @@
         <v>61</v>
       </c>
       <c r="C141" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E141" s="3">
         <v>1.05008077544426E-2</v>
@@ -11572,10 +11572,10 @@
         <v>63</v>
       </c>
       <c r="C142" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E142" s="3">
         <v>10.4051967276221</v>
@@ -11649,10 +11649,10 @@
         <v>65</v>
       </c>
       <c r="C143" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E143" s="3">
         <v>0.22697899838449101</v>
@@ -11726,10 +11726,10 @@
         <v>67</v>
       </c>
       <c r="C144" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E144" s="3">
         <v>0.83868782267558195</v>
@@ -11803,10 +11803,10 @@
         <v>69</v>
       </c>
       <c r="C145" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E145" s="3">
         <v>0.70147318557327598</v>
@@ -11880,10 +11880,10 @@
         <v>71</v>
       </c>
       <c r="C146" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E146" s="3">
         <v>-0.576828754391154</v>
@@ -11957,10 +11957,10 @@
         <v>72</v>
       </c>
       <c r="C147" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E147" s="3">
         <v>0.15589660743134101</v>
@@ -12034,10 +12034,10 @@
         <v>73</v>
       </c>
       <c r="C148" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E148" s="3">
         <v>0.149434571890145</v>
@@ -12111,10 +12111,10 @@
         <v>75</v>
       </c>
       <c r="C149" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E149" s="3">
         <v>0.35298869143780298</v>
@@ -12188,10 +12188,10 @@
         <v>77</v>
       </c>
       <c r="C150" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E150" s="3">
         <v>0.50969305331179304</v>
@@ -12265,10 +12265,10 @@
         <v>79</v>
       </c>
       <c r="C151" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E151" s="3">
         <v>0.133279483037157</v>
@@ -12342,10 +12342,10 @@
         <v>23</v>
       </c>
       <c r="C152" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E152" s="3">
         <v>2.3809523809523799E-3</v>
@@ -12419,10 +12419,10 @@
         <v>25</v>
       </c>
       <c r="C153" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E153" s="3">
         <v>4.88505515906986E-2</v>
@@ -12496,10 +12496,10 @@
         <v>27</v>
       </c>
       <c r="C154" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E154" s="3">
         <v>7.40369243494915</v>
@@ -12573,10 +12573,10 @@
         <v>29</v>
       </c>
       <c r="C155" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E155" s="3">
         <v>8.6507936507936506E-2</v>
@@ -12650,10 +12650,10 @@
         <v>31</v>
       </c>
       <c r="C156" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E156" s="3">
         <v>8.8833333333333293</v>
@@ -12727,10 +12727,10 @@
         <v>33</v>
       </c>
       <c r="C157" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E157" s="3">
         <v>35.012698412698398</v>
@@ -12804,10 +12804,10 @@
         <v>35</v>
       </c>
       <c r="C158" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E158" s="3">
         <v>4.5238095238095202E-2</v>
@@ -12881,10 +12881,10 @@
         <v>37</v>
       </c>
       <c r="C159" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E159" s="3">
         <v>0.95476190476190503</v>
@@ -12958,10 +12958,10 @@
         <v>39</v>
       </c>
       <c r="C160" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E160" s="3">
         <v>0</v>
@@ -13035,10 +13035,10 @@
         <v>41</v>
       </c>
       <c r="C161" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E161" s="3">
         <v>4.36507936507936E-2</v>
@@ -13112,10 +13112,10 @@
         <v>43</v>
       </c>
       <c r="C162" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E162" s="3">
         <v>8.4901470702052798E-2</v>
@@ -13189,10 +13189,10 @@
         <v>45</v>
       </c>
       <c r="C163" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E163" s="3">
         <v>7.9365079365079398E-4</v>
@@ -13266,10 +13266,10 @@
         <v>47</v>
       </c>
       <c r="C164" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E164" s="3">
         <v>12.634376028892399</v>
@@ -13343,10 +13343,10 @@
         <v>49</v>
       </c>
       <c r="C165" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E165" s="3">
         <v>45.547619047619101</v>
@@ -13420,10 +13420,10 @@
         <v>51</v>
       </c>
       <c r="C166" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E166" s="3">
         <v>3.36061512585729E-2</v>
@@ -13497,10 +13497,10 @@
         <v>53</v>
       </c>
       <c r="C167" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E167" s="3">
         <v>0.12705897091451801</v>
@@ -13574,10 +13574,10 @@
         <v>55</v>
       </c>
       <c r="C168" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E168" s="3">
         <v>139.228487800322</v>
@@ -13651,10 +13651,10 @@
         <v>57</v>
       </c>
       <c r="C169" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E169" s="3">
         <v>0.94365079365079396</v>
@@ -13728,10 +13728,10 @@
         <v>59</v>
       </c>
       <c r="C170" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E170" s="3">
         <v>0.32936507936507903</v>
@@ -13805,10 +13805,10 @@
         <v>61</v>
       </c>
       <c r="C171" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E171" s="3">
         <v>2.3809523809523799E-3</v>
@@ -13882,10 +13882,10 @@
         <v>63</v>
       </c>
       <c r="C172" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E172" s="3">
         <v>8.1746907121960106</v>
@@ -13959,10 +13959,10 @@
         <v>65</v>
       </c>
       <c r="C173" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E173" s="3">
         <v>0.167460317460317</v>
@@ -14036,10 +14036,10 @@
         <v>67</v>
       </c>
       <c r="C174" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E174" s="3">
         <v>0.87585192664511602</v>
@@ -14113,10 +14113,10 @@
         <v>69</v>
       </c>
       <c r="C175" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E175" s="3">
         <v>0.60992479125510801</v>
@@ -14190,10 +14190,10 @@
         <v>71</v>
       </c>
       <c r="C176" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E176" s="3">
         <v>-0.48519741496485103</v>
@@ -14267,10 +14267,10 @@
         <v>72</v>
       </c>
       <c r="C177" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E177" s="3">
         <v>8.6507936507936506E-2</v>
@@ -14344,10 +14344,10 @@
         <v>73</v>
       </c>
       <c r="C178" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E178" s="3">
         <v>0.12460317460317499</v>
@@ -14421,10 +14421,10 @@
         <v>75</v>
       </c>
       <c r="C179" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E179" s="3">
         <v>0.24047619047619001</v>
@@ -14498,10 +14498,10 @@
         <v>77</v>
       </c>
       <c r="C180" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E180" s="3">
         <v>0.61349206349206398</v>
@@ -14575,10 +14575,10 @@
         <v>79</v>
       </c>
       <c r="C181" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E181" s="3">
         <v>0.142063492063492</v>
@@ -14652,10 +14652,10 @@
         <v>23</v>
       </c>
       <c r="C182" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E182" s="3">
         <v>2.50403877221325E-2</v>
@@ -14729,10 +14729,10 @@
         <v>25</v>
       </c>
       <c r="C183" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E183" s="3">
         <v>0.24420096107174599</v>
@@ -14806,10 +14806,10 @@
         <v>27</v>
       </c>
       <c r="C184" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E184" s="3">
         <v>17.2827986387449</v>
@@ -14883,10 +14883,10 @@
         <v>29</v>
       </c>
       <c r="C185" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E185" s="3">
         <v>0.36106623586429698</v>
@@ -14960,10 +14960,10 @@
         <v>31</v>
       </c>
       <c r="C186" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E186" s="3">
         <v>8.1696284329563795</v>
@@ -15037,10 +15037,10 @@
         <v>33</v>
       </c>
       <c r="C187" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E187" s="3">
         <v>36.853796445880398</v>
@@ -15114,10 +15114,10 @@
         <v>35</v>
       </c>
       <c r="C188" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E188" s="3">
         <v>0.56946688206785101</v>
@@ -15191,10 +15191,10 @@
         <v>37</v>
       </c>
       <c r="C189" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E189" s="3">
         <v>0.86833602584814196</v>
@@ -15268,10 +15268,10 @@
         <v>39</v>
       </c>
       <c r="C190" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E190" s="3">
         <v>1.53473344103393E-2</v>
@@ -15345,10 +15345,10 @@
         <v>41</v>
       </c>
       <c r="C191" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E191" s="3">
         <v>0.104200323101777</v>
@@ -15422,10 +15422,10 @@
         <v>43</v>
       </c>
       <c r="C192" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E192" s="3">
         <v>3.3784575296019699E-2</v>
@@ -15499,10 +15499,10 @@
         <v>45</v>
       </c>
       <c r="C193" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E193" s="3">
         <v>1.77705977382876E-2</v>
@@ -15576,10 +15576,10 @@
         <v>47</v>
       </c>
       <c r="C194" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E194" s="3">
         <v>15.8419245170743</v>
@@ -15653,10 +15653,10 @@
         <v>49</v>
       </c>
       <c r="C195" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E195" s="3">
         <v>60.835218093699503</v>
@@ -15730,10 +15730,10 @@
         <v>51</v>
       </c>
       <c r="C196" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E196" s="3">
         <v>6.3327752301990003E-2</v>
@@ -15807,10 +15807,10 @@
         <v>53</v>
       </c>
       <c r="C197" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E197" s="3">
         <v>2.0673222382258001E-2</v>
@@ -15884,10 +15884,10 @@
         <v>55</v>
       </c>
       <c r="C198" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E198" s="3">
         <v>431.05428028114198</v>
@@ -15961,10 +15961,10 @@
         <v>57</v>
       </c>
       <c r="C199" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E199" s="3">
         <v>0.80856219709208399</v>
@@ -16038,10 +16038,10 @@
         <v>59</v>
       </c>
       <c r="C200" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E200" s="3">
         <v>0.41437802907915999</v>
@@ -16115,10 +16115,10 @@
         <v>61</v>
       </c>
       <c r="C201" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E201" s="3">
         <v>5.5735056542811003E-2</v>
@@ -16192,10 +16192,10 @@
         <v>63</v>
       </c>
       <c r="C202" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E202" s="3">
         <v>20.831162396415198</v>
@@ -16269,10 +16269,10 @@
         <v>65</v>
       </c>
       <c r="C203" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E203" s="3">
         <v>0.24636510500807801</v>
@@ -16346,10 +16346,10 @@
         <v>67</v>
       </c>
       <c r="C204" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E204" s="3">
         <v>0.93057411345645702</v>
@@ -16423,10 +16423,10 @@
         <v>69</v>
       </c>
       <c r="C205" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E205" s="3">
         <v>0.82574545193135596</v>
@@ -16500,10 +16500,10 @@
         <v>71</v>
       </c>
       <c r="C206" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E206" s="3">
         <v>-0.42175762464709099</v>
@@ -16577,10 +16577,10 @@
         <v>72</v>
       </c>
       <c r="C207" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E207" s="3">
         <v>0.25686591276252002</v>
@@ -16654,10 +16654,10 @@
         <v>73</v>
       </c>
       <c r="C208" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E208" s="3">
         <v>0.30129240710823901</v>
@@ -16731,10 +16731,10 @@
         <v>75</v>
       </c>
       <c r="C209" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E209" s="3">
         <v>0.327140549273021</v>
@@ -16808,10 +16808,10 @@
         <v>77</v>
       </c>
       <c r="C210" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E210" s="3">
         <v>0.36510500807754398</v>
@@ -16885,10 +16885,10 @@
         <v>79</v>
       </c>
       <c r="C211" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E211" s="3">
         <v>0.302907915993538</v>

</xml_diff>